<commit_message>
Modified excel template specification
</commit_message>
<xml_diff>
--- a/uesgraphs/data/uesgraphs_parameters_template.xlsx
+++ b/uesgraphs/data/uesgraphs_parameters_template.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27932"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rka-lko\git\uesgraphs\uesgraphs\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99E88F7-FAC8-454C-9AF0-63C23F879A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="INFO"/>
-    <sheet r:id="rId2" sheetId="2" name="Simulation"/>
-    <sheet r:id="rId3" sheetId="3" name="Demands"/>
-    <sheet r:id="rId4" sheetId="4" name="Supply"/>
-    <sheet r:id="rId5" sheetId="5" name="Pipes"/>
-    <sheet r:id="rId6" sheetId="6" name="Individual_Parameters"/>
+    <sheet name="INFO" sheetId="1" r:id="rId1"/>
+    <sheet name="Simulation" sheetId="2" r:id="rId2"/>
+    <sheet name="Demands" sheetId="3" r:id="rId3"/>
+    <sheet name="Supply" sheetId="4" r:id="rId4"/>
+    <sheet name="Pipes" sheetId="5" r:id="rId5"/>
+    <sheet name="Individual_Parameters" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="184">
   <si>
     <t>OPTIONAL FEATURE - Individual Node/Edge Parameters</t>
   </si>
@@ -315,9 +321,6 @@
     <t>m_flow_nominal</t>
   </si>
   <si>
-    <t>AUTO</t>
-  </si>
-  <si>
     <t>kg/s</t>
   </si>
   <si>
@@ -366,9 +369,6 @@
     <t>Q_flow_nominal</t>
   </si>
   <si>
-    <t>OpenLoop_VarTSupplyDp</t>
-  </si>
-  <si>
     <t>Nominal heat flow rate added to medium</t>
   </si>
   <si>
@@ -568,13 +568,21 @@
   </si>
   <si>
     <t>For more information, see: https://github.com/RWTH-EBC/uesgraphs</t>
+  </si>
+  <si>
+    <t>Templates</t>
+  </si>
+  <si>
+    <t>OpenLoop_VarTSupplyDp, OpenLoop_VarTSupplyDpBypass</t>
+  </si>
+  <si>
+    <t>DHCSubstationHeatPumpChiller, DHCSubstationHeatPumpDirectCooling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -585,13 +593,13 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFffffff"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -615,7 +623,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF0000ff"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -639,7 +647,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFffffff"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -680,16 +688,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -757,101 +765,106 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="33">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="10" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -862,10 +875,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -903,71 +916,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -995,7 +1008,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1018,11 +1031,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1031,13 +1044,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1047,7 +1060,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1056,7 +1069,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1065,7 +1078,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1073,10 +1086,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1141,25 +1154,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:F27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="2.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="50.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="2.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="2" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1167,27 +1181,27 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="27">
+    <row r="2" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="B2" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="24" t="s">
-        <v>151</v>
+      <c r="B3" s="23" t="s">
+        <v>149</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1195,27 +1209,27 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="5" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="6">
+      <c r="B5" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+    </row>
+    <row r="6" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="B6" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1223,101 +1237,101 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21">
+    <row r="8" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="25" t="s">
-        <v>154</v>
+      <c r="B8" s="24" t="s">
+        <v>152</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
+    <row r="9" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>155</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>157</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>158</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>160</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="D11" s="27" t="s">
+      <c r="B11" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>160</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>158</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>160</v>
+      <c r="B12" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>158</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>160</v>
+      <c r="B13" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>158</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="D14" s="26" t="s">
         <v>167</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>169</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1325,127 +1339,127 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="21.75">
+    <row r="16" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="25" t="s">
-        <v>170</v>
+      <c r="B16" s="24" t="s">
+        <v>168</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="17" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+    </row>
+    <row r="18" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A18" s="7"/>
-      <c r="B18" s="5" t="s">
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A19" s="7"/>
-      <c r="B19" s="5" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A20" s="7"/>
-      <c r="B20" s="5" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+    </row>
+    <row r="22" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A21" s="7"/>
-      <c r="B21" s="5" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+    </row>
+    <row r="23" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="24" t="s">
         <v>175</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A22" s="7"/>
-      <c r="B22" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="21.75">
-      <c r="A23" s="2"/>
-      <c r="B23" s="25" t="s">
-        <v>177</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="24" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+    </row>
+    <row r="25" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+    </row>
+    <row r="26" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A25" s="7"/>
-      <c r="B25" s="5" t="s">
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+    </row>
+    <row r="27" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A26" s="7"/>
-      <c r="B26" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A27" s="7"/>
-      <c r="B27" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+    </row>
+    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1453,7 +1467,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1461,57 +1475,58 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="B30" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B24:F24"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="80.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="90.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="90" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -1525,79 +1540,79 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="2" spans="1:4" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A3" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>135</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B4" s="15">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="B5" s="15">
         <v>86400</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A6" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="6">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>60</v>
@@ -1606,21 +1621,21 @@
         <v>61</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A8" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>148</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1629,26 +1644,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="80.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="90.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="90" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>33</v>
       </c>
@@ -1658,12 +1674,14 @@
       <c r="C1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="19" t="s">
+        <v>181</v>
+      </c>
       <c r="E1" s="21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -1678,7 +1696,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
@@ -1693,7 +1711,7 @@
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>83</v>
       </c>
@@ -1708,7 +1726,7 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>86</v>
       </c>
@@ -1723,7 +1741,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>88</v>
       </c>
@@ -1738,12 +1756,12 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B7" s="14">
-        <v>316.15</v>
+        <v>316.14999999999998</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>73</v>
@@ -1753,12 +1771,12 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B8" s="14">
-        <v>302.15</v>
+        <v>302.14999999999998</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>73</v>
@@ -1768,7 +1786,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>94</v>
       </c>
@@ -1783,24 +1801,22 @@
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="10" spans="1:5" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>99</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="B11" s="18">
         <v>20</v>
@@ -1809,15 +1825,15 @@
         <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="7" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="B12" s="18">
         <v>10</v>
@@ -1826,15 +1842,15 @@
         <v>73</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="B13" s="18">
         <v>30</v>
@@ -1843,15 +1859,15 @@
         <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E13" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="B14" s="18">
         <v>10</v>
@@ -1860,15 +1876,15 @@
         <v>73</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="B15" s="18">
         <v>100000</v>
@@ -1877,30 +1893,30 @@
         <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
       <c r="E15" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="B16" s="18">
         <v>-10000</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="B17" s="18">
         <v>1000</v>
@@ -1909,15 +1925,15 @@
         <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="B18" s="18">
         <v>10</v>
@@ -1925,14 +1941,14 @@
       <c r="C18" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>115</v>
+      <c r="D18" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>72</v>
       </c>
@@ -1942,33 +1958,33 @@
       <c r="C19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>115</v>
+      <c r="D19" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B20" s="18">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="B21" s="18">
         <v>328.15</v>
@@ -1977,15 +1993,15 @@
         <v>73</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="B22" s="18">
         <v>15</v>
@@ -1994,25 +2010,25 @@
         <v>73</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E22" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A23" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>129</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>61</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2021,26 +2037,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="80.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="90.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="90" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -2050,12 +2067,14 @@
       <c r="C1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="19" t="s">
+        <v>181</v>
+      </c>
       <c r="E1" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -2070,7 +2089,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
@@ -2085,7 +2104,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
@@ -2100,7 +2119,7 @@
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>67</v>
       </c>
@@ -2117,12 +2136,12 @@
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B6" s="18">
-        <v>313.15</v>
+        <v>313.14999999999998</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>73</v>
@@ -2134,7 +2153,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>75</v>
       </c>
@@ -2151,7 +2170,7 @@
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="8" spans="1:5" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>59</v>
       </c>
@@ -2172,25 +2191,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="80.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="90.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="90" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
@@ -2204,7 +2224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="2" spans="1:4" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -2218,7 +2238,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="3" spans="1:4" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
@@ -2232,7 +2252,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -2246,7 +2266,7 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -2260,7 +2280,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
@@ -2274,7 +2294,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
@@ -2288,7 +2308,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -2302,7 +2322,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="9" spans="1:4" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>56</v>
       </c>
@@ -2316,7 +2336,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="10" spans="1:4" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>59</v>
       </c>
@@ -2336,7 +2356,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2344,17 +2364,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="60.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="18" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2364,7 +2384,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2374,7 +2394,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2384,7 +2404,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2392,7 +2412,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2412,7 +2432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -2432,7 +2452,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -2452,7 +2472,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -2472,7 +2492,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -2492,7 +2512,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="10" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -2500,7 +2520,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
@@ -2510,7 +2530,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="12" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
@@ -2520,7 +2540,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="13" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
@@ -2530,7 +2550,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="14" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>30</v>
       </c>
@@ -2540,7 +2560,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="15" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>31</v>
       </c>
@@ -2550,7 +2570,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row r="16" spans="1:6" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Modified excel and create docs
</commit_message>
<xml_diff>
--- a/uesgraphs/data/uesgraphs_parameters_template.xlsx
+++ b/uesgraphs/data/uesgraphs_parameters_template.xlsx
@@ -1553,17 +1553,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="65.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,6 +1932,9 @@
       <c r="E24" s="0" t="s">
         <v>124</v>
       </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1956,7 +1957,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2081,7 +2082,7 @@
         <v>139</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Cleaning of model gen example
</commit_message>
<xml_diff>
--- a/uesgraphs/data/uesgraphs_parameters_template.xlsx
+++ b/uesgraphs/data/uesgraphs_parameters_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="INFO"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="198">
   <si>
     <t>OPTIONAL FEATURE - Individual Node/Edge Parameters</t>
   </si>
@@ -462,6 +462,9 @@
     <t>Simulation stop time (86400s = 24h)</t>
   </si>
   <si>
+    <t>timestep</t>
+  </si>
+  <si>
     <t>tolerance</t>
   </si>
   <si>
@@ -484,6 +487,24 @@
   </si>
   <si>
     <t>Medium definition: AixLib.Media.Water, AixLib.Media.Specialized.Water.ConstantProperties_pT, AixLib.Media.Antifreeze.PropyleneGlycolWater</t>
+  </si>
+  <si>
+    <t>p_nominal</t>
+  </si>
+  <si>
+    <t>Nominal pressure of medium</t>
+  </si>
+  <si>
+    <t>T_nominal</t>
+  </si>
+  <si>
+    <t>Nominal temperature of medium</t>
+  </si>
+  <si>
+    <t>fraction_glycol</t>
+  </si>
+  <si>
+    <t>Fraction of glycol if water-glycol medium is used</t>
   </si>
   <si>
     <t>1.0 m</t>
@@ -1192,7 +1213,7 @@
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2"/>
       <c r="B2" s="21" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
@@ -1202,7 +1223,7 @@
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2"/>
       <c r="B3" s="22" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1220,7 +1241,7 @@
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2"/>
       <c r="B5" s="4" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1230,7 +1251,7 @@
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2"/>
       <c r="B6" s="4" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1248,7 +1269,7 @@
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2"/>
       <c r="B8" s="23" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1258,13 +1279,13 @@
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2"/>
       <c r="B9" s="24" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1272,13 +1293,13 @@
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1286,13 +1307,13 @@
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2"/>
       <c r="B11" s="25" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1300,13 +1321,13 @@
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="2"/>
       <c r="B12" s="25" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1314,13 +1335,13 @@
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="2"/>
       <c r="B13" s="25" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1328,13 +1349,13 @@
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="2"/>
       <c r="B14" s="25" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1350,7 +1371,7 @@
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="2"/>
       <c r="B16" s="23" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1360,7 +1381,7 @@
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="2"/>
       <c r="B17" s="4" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1370,7 +1391,7 @@
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="2"/>
       <c r="B18" s="4" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1380,7 +1401,7 @@
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="2"/>
       <c r="B19" s="4" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1390,7 +1411,7 @@
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="2"/>
       <c r="B20" s="4" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1400,7 +1421,7 @@
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1410,7 +1431,7 @@
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="2"/>
       <c r="B22" s="4" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1420,7 +1441,7 @@
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="2"/>
       <c r="B23" s="23" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1430,7 +1451,7 @@
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="2"/>
       <c r="B24" s="4" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1440,7 +1461,7 @@
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="2"/>
       <c r="B25" s="4" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1450,7 +1471,7 @@
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="2"/>
       <c r="B26" s="4" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1460,7 +1481,7 @@
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="2"/>
       <c r="B27" s="4" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -1486,7 +1507,7 @@
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="2"/>
       <c r="B30" s="26" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
@@ -1519,9 +1540,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
@@ -1604,59 +1625,113 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="B6" s="20">
+        <v>900</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>151</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="20">
+        <v>400000</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="20">
+        <v>353</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B12" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>157</v>
+      <c r="B13" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2292,7 +2367,7 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>

</xml_diff>